<commit_message>
updates to tidy code
</commit_message>
<xml_diff>
--- a/data/vaccine_allocation_strategies_income_group.xlsx
+++ b/data/vaccine_allocation_strategies_income_group.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Alexandra\covid_vaccine_allocation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C039CE1-3D68-4EDD-89B4-427B641EA322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{307939B8-4239-4F41-AE3E-DE406854B31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="income_group_summary_cov1" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="49">
   <si>
     <t>World Bank Income Group</t>
   </si>
@@ -166,6 +166,18 @@
   </si>
   <si>
     <t>Strategy5</t>
+  </si>
+  <si>
+    <t>old_middle</t>
+  </si>
+  <si>
+    <t>weighted doses of 1.1 b (less 15%, divided by 2) doses acros MIC</t>
+  </si>
+  <si>
+    <t>All countries receive doses in proportion to population - 2 dose schedule - allocated to elderly and then middle</t>
+  </si>
+  <si>
+    <t>All countries receive doses in proportion to number of people aged 65+ in population - allocated to elderly and then middle</t>
   </si>
 </sst>
 </file>
@@ -690,7 +702,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -703,7 +715,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="35" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -711,6 +722,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1068,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9D2C4C-BC5D-408C-B7F4-CF07B36A42B2}">
-  <dimension ref="A1:O62"/>
+  <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,17 +1108,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1142,8 +1157,8 @@
       <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="O2" t="s">
-        <v>21</v>
+      <c r="O2" s="19" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -1191,6 +1206,7 @@
         <f>L3/SUM(F3:H3)</f>
         <v>0.11116275712463609</v>
       </c>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1238,8 +1254,8 @@
         <v>0.11116275712463609</v>
       </c>
       <c r="O4">
-        <f>1.1*SUM(F4:H4)/SUM(F4:H5)*0.85</f>
-        <v>0.4628405308448143</v>
+        <f>1.1*SUM(F4:H4)/SUM(F4:H5)*0.85/2</f>
+        <v>0.23142026542240715</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -1288,8 +1304,8 @@
         <v>0.11116275712463611</v>
       </c>
       <c r="O5">
-        <f>1.1*SUM(F5:H5)/SUM(F4:H5)*0.85</f>
-        <v>0.47215946915518575</v>
+        <f>1.1*SUM(F5:H5)/SUM(F4:H5)*0.85/2</f>
+        <v>0.23607973457759288</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -1409,7 +1425,7 @@
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <f>E11*$B$8*1000000000</f>
         <v>134758363.60022315</v>
       </c>
@@ -1421,7 +1437,7 @@
         <f>IF(G11&gt;F11,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I11" s="17">
+      <c r="I11" s="16">
         <f>F11</f>
         <v>134758363.60022315</v>
       </c>
@@ -1447,7 +1463,7 @@
         <f t="shared" ref="E12:E14" si="3">K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f>E12*$B$8*1000000000</f>
         <v>317465581.59489292</v>
       </c>
@@ -1459,7 +1475,7 @@
         <f>IF(G12&gt;F12,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I12" s="17">
+      <c r="I12" s="16">
         <f t="shared" ref="I12:I14" si="4">F12</f>
         <v>317465581.59489292</v>
       </c>
@@ -1485,7 +1501,7 @@
         <f t="shared" si="3"/>
         <v>0.38100883182298734</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <f>E13*$B$8*1000000000</f>
         <v>323857507.04953927</v>
       </c>
@@ -1497,7 +1513,7 @@
         <f>IF(G13&gt;F13,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I13" s="17">
+      <c r="I13" s="16">
         <f t="shared" si="4"/>
         <v>323857507.04953927</v>
       </c>
@@ -1523,7 +1539,7 @@
         <f t="shared" si="3"/>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <f>E14*$B$8*1000000000</f>
         <v>73918547.755344689</v>
       </c>
@@ -1535,7 +1551,7 @@
         <f>IF(G14&gt;F14,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="16">
         <f t="shared" si="4"/>
         <v>73918547.755344689</v>
       </c>
@@ -1552,12 +1568,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1587,1102 +1603,844 @@
       </c>
       <c r="K18" s="9"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>0.8</v>
       </c>
       <c r="D19" s="7">
-        <f>H3</f>
-        <v>0.25821176254799999</v>
+        <f>G3+H3</f>
+        <v>1.0376960973759999</v>
       </c>
       <c r="E19" s="8">
         <f>E11</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <f>E19*$B$16*1000000000</f>
         <v>134758363.60022315</v>
       </c>
       <c r="G19" s="11">
         <f>C19*D19*1000000000</f>
-        <v>206569410.03840002</v>
+        <v>830156877.90079999</v>
       </c>
       <c r="H19" t="str">
         <f>IF(G19&gt;F19,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="16">
         <f>F19</f>
         <v>134758363.60022315</v>
       </c>
       <c r="K19" s="9">
         <f>I19/G19*0.8</f>
-        <v>0.52189087851941829</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.12986303402410759</v>
+      </c>
+      <c r="L19" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>0.8</v>
       </c>
       <c r="D20" s="7">
-        <f>H4</f>
-        <v>0.27987455332200001</v>
+        <f t="shared" ref="D20:D22" si="5">G4+H4</f>
+        <v>2.1761674452180002</v>
       </c>
       <c r="E20" s="8">
         <f>E12</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f>E20*$B$16*1000000000</f>
         <v>317465581.59489292</v>
       </c>
       <c r="G20" s="11">
         <f>C20*D20*1000000000</f>
-        <v>223899642.65760002</v>
+        <v>1740933956.1744001</v>
       </c>
       <c r="H20" t="str">
         <f>IF(G20&gt;F20,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I20" s="17">
-        <f>G20</f>
-        <v>223899642.65760002</v>
+        <v>N</v>
+      </c>
+      <c r="I20" s="16">
+        <f t="shared" ref="I20:I22" si="6">F20</f>
+        <v>317465581.59489292</v>
       </c>
       <c r="K20" s="9">
         <f>I20/G20*0.8</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.14588288336566421</v>
+      </c>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>0.8</v>
       </c>
       <c r="D21" s="7">
-        <f>H5</f>
-        <v>0.16606171328700001</v>
+        <f t="shared" si="5"/>
+        <v>2.0539211906549997</v>
       </c>
       <c r="E21" s="8">
         <f>E13</f>
         <v>0.38100883182298734</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <f>E21*$B$16*1000000000</f>
         <v>323857507.04953927</v>
       </c>
       <c r="G21" s="11">
         <f>C21*D21*1000000000</f>
-        <v>132849370.6296</v>
+        <v>1643136952.5239999</v>
       </c>
       <c r="H21" t="str">
         <f>IF(G21&gt;F21,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I21" s="17">
-        <f t="shared" ref="I21:I22" si="5">G21</f>
-        <v>132849370.6296</v>
+        <v>N</v>
+      </c>
+      <c r="I21" s="16">
+        <f t="shared" si="6"/>
+        <v>323857507.04953927</v>
       </c>
       <c r="K21" s="9">
         <f>I21/G21*0.8</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.15767766968033492</v>
+      </c>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C22">
         <v>0.8</v>
       </c>
       <c r="D22" s="7">
-        <f>H6</f>
-        <v>2.0613693288000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.398309750952</v>
       </c>
       <c r="E22" s="8">
         <f>E14</f>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <f>E22*$B$16*1000000000</f>
         <v>73918547.755344689</v>
       </c>
       <c r="G22" s="11">
         <f>C22*D22*1000000000</f>
-        <v>16490954.630400002</v>
+        <v>318647800.76160002</v>
       </c>
       <c r="H22" t="str">
         <f>IF(G22&gt;F22,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I22" s="17">
-        <f t="shared" si="5"/>
-        <v>16490954.630400002</v>
+        <v>N</v>
+      </c>
+      <c r="I22" s="16">
+        <f t="shared" si="6"/>
+        <v>73918547.755344689</v>
       </c>
       <c r="K22" s="9">
         <f>I22/G22*0.8</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23">
-        <v>0.8</v>
-      </c>
-      <c r="D23" s="7">
-        <f>G3</f>
-        <v>0.77948433482799995</v>
-      </c>
-      <c r="E23" s="8">
-        <f>E11</f>
-        <v>0.15853925129438018</v>
-      </c>
-      <c r="F23" s="13">
-        <v>0</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="I23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24">
-        <v>0.8</v>
-      </c>
-      <c r="D24" s="7">
-        <f>G4</f>
-        <v>1.8962928918960003</v>
-      </c>
-      <c r="E24" s="8">
-        <f t="shared" ref="E24:E26" si="6">E12</f>
-        <v>0.37348891952340341</v>
-      </c>
-      <c r="F24" s="13">
-        <f>F20-G20</f>
-        <v>93565938.937292904</v>
-      </c>
-      <c r="G24" s="11">
-        <f>C24*D24*1000000000</f>
-        <v>1517034313.5168004</v>
-      </c>
-      <c r="I24" s="17">
-        <f>F24</f>
-        <v>93565938.937292904</v>
-      </c>
-      <c r="K24" s="9">
-        <f>I24/G24*0.8</f>
-        <v>4.934150169372907E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25">
-        <v>0.8</v>
-      </c>
-      <c r="D25" s="7">
-        <f>G5</f>
-        <v>1.8878594773679997</v>
-      </c>
-      <c r="E25" s="8">
-        <f t="shared" si="6"/>
-        <v>0.38100883182298734</v>
-      </c>
-      <c r="F25" s="13">
-        <f>F21-G21</f>
-        <v>191008136.41993928</v>
-      </c>
-      <c r="G25" s="11">
-        <f>C25*D25*1000000000</f>
-        <v>1510287581.8943999</v>
-      </c>
-      <c r="I25" s="17">
-        <f t="shared" ref="I25:I26" si="7">F25</f>
-        <v>191008136.41993928</v>
-      </c>
-      <c r="K25" s="9">
-        <f>I25/G25*0.8</f>
-        <v>0.10117709432814218</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+        <v>0.1855805628124142</v>
+      </c>
+      <c r="L22" s="7"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C26">
         <v>0.8</v>
       </c>
-      <c r="D26" s="7">
-        <f>G6</f>
-        <v>0.377696057664</v>
-      </c>
-      <c r="E26" s="8">
-        <f t="shared" si="6"/>
-        <v>8.6962997359229049E-2</v>
-      </c>
-      <c r="F26" s="13">
-        <f>F22-G22</f>
-        <v>57427593.124944687</v>
-      </c>
-      <c r="G26" s="11">
-        <f>C26*D26*1000000000</f>
-        <v>302156846.13120002</v>
-      </c>
-      <c r="I26" s="17">
+      <c r="D26" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="7">
+        <f>C19</f>
+        <v>0.8</v>
+      </c>
+      <c r="D27" s="7">
+        <f>D19</f>
+        <v>1.0376960973759999</v>
+      </c>
+      <c r="E27" s="8">
+        <f>H3/SUM($H$3:$H$6)</f>
+        <v>0.35627124688223982</v>
+      </c>
+      <c r="F27" s="12">
+        <f>E27*$B$16*1000000000</f>
+        <v>302830559.84990388</v>
+      </c>
+      <c r="G27" s="11">
+        <f>C27*D27*1000000000</f>
+        <v>830156877.90079999</v>
+      </c>
+      <c r="H27" t="str">
+        <f>IF(G27&gt;F27,"N", "Y")</f>
+        <v>N</v>
+      </c>
+      <c r="I27" s="16">
+        <f t="shared" ref="I27:I30" si="7">F27</f>
+        <v>302830559.84990388</v>
+      </c>
+      <c r="K27" s="9">
+        <f>I27/G27*0.8</f>
+        <v>0.29182971836905341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="7">
+        <f>C20</f>
+        <v>0.8</v>
+      </c>
+      <c r="D28" s="7">
+        <f>D20</f>
+        <v>2.1761674452180002</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" ref="E28:E30" si="8">H4/SUM($H$3:$H$6)</f>
+        <v>0.38616078175022389</v>
+      </c>
+      <c r="F28" s="12">
+        <f>E28*$B$16*1000000000</f>
+        <v>328236664.48769027</v>
+      </c>
+      <c r="G28" s="11">
+        <f>C28*D28*1000000000</f>
+        <v>1740933956.1744001</v>
+      </c>
+      <c r="H28" t="str">
+        <f>IF(G28&gt;F28,"N", "Y")</f>
+        <v>N</v>
+      </c>
+      <c r="I28" s="16">
         <f t="shared" si="7"/>
-        <v>57427593.124944687</v>
-      </c>
-      <c r="K26" s="9">
-        <f>I26/G26*0.8</f>
-        <v>0.15204710761379595</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+        <v>328236664.48769027</v>
+      </c>
+      <c r="K28" s="9">
+        <f t="shared" ref="K28:K30" si="9">I28/G28*0.8</f>
+        <v>0.15083244867437523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="7">
+        <f>C21</f>
+        <v>0.8</v>
+      </c>
+      <c r="D29" s="7">
+        <f>D21</f>
+        <v>2.0539211906549997</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" si="8"/>
+        <v>0.22912594325040658</v>
+      </c>
+      <c r="F29" s="12">
+        <f>E29*$B$16*1000000000</f>
+        <v>194757051.76284558</v>
+      </c>
+      <c r="G29" s="11">
+        <f>C29*D29*1000000000</f>
+        <v>1643136952.5239999</v>
+      </c>
+      <c r="H29" t="str">
+        <f>IF(G29&gt;F29,"N", "Y")</f>
+        <v>N</v>
+      </c>
+      <c r="I29" s="16">
+        <f t="shared" si="7"/>
+        <v>194757051.76284558</v>
+      </c>
+      <c r="K29" s="9">
+        <f t="shared" si="9"/>
+        <v>9.4822066517915971E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="7">
+        <f>C22</f>
+        <v>0.8</v>
+      </c>
+      <c r="D30" s="7">
+        <f>D22</f>
+        <v>0.398309750952</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="8"/>
+        <v>2.8442028117129644E-2</v>
+      </c>
+      <c r="F30" s="12">
+        <f>E30*$B$16*1000000000</f>
+        <v>24175723.899560198</v>
+      </c>
+      <c r="G30" s="11">
+        <f>C30*D30*1000000000</f>
+        <v>318647800.76160002</v>
+      </c>
+      <c r="H30" t="str">
+        <f>IF(G30&gt;F30,"N", "Y")</f>
+        <v>N</v>
+      </c>
+      <c r="I30" s="16">
+        <f t="shared" si="7"/>
+        <v>24175723.899560198</v>
+      </c>
+      <c r="K30" s="9">
+        <f t="shared" si="9"/>
+        <v>6.0695787240402248E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B28">
+      <c r="B32">
         <v>0.85</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>13</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B34" t="s">
         <v>14</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C34" t="s">
         <v>15</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D34" t="s">
         <v>33</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E34" t="s">
         <v>28</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F34" t="s">
         <v>38</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G34" t="s">
         <v>34</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H34" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>4</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B35" t="s">
         <v>12</v>
       </c>
-      <c r="C31">
+      <c r="C35">
         <v>0.8</v>
       </c>
-      <c r="D31" s="7">
+      <c r="D35" s="7">
         <f>SUM(F3:H3)</f>
         <v>1.2122617959999999</v>
       </c>
-      <c r="E31">
-        <f>B28</f>
+      <c r="E35">
+        <f>B32</f>
         <v>0.85</v>
       </c>
-      <c r="F31" s="12">
-        <f>E31*1000000000</f>
+      <c r="F35" s="12">
+        <f>E35*1000000000</f>
         <v>850000000</v>
       </c>
-      <c r="G31" s="7">
-        <f>C31*D31*1000000000</f>
+      <c r="G35" s="7">
+        <f>C35*D35*1000000000</f>
         <v>969809436.79999995</v>
       </c>
-      <c r="H31" t="str">
-        <f>IF(G31&gt;F31,"N", "Y")</f>
+      <c r="H35" t="str">
+        <f>IF(G35&gt;F35,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I31">
-        <f>F31</f>
+      <c r="I35" s="11">
+        <f>F35</f>
         <v>850000000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
-      <c r="C32">
+      <c r="C36">
         <v>1</v>
       </c>
-      <c r="D32">
+      <c r="D36">
         <v>0</v>
       </c>
-      <c r="E32">
-        <f>C32*D32</f>
+      <c r="E36">
+        <f>C36*D36</f>
         <v>0</v>
       </c>
-      <c r="F32" s="12">
+      <c r="F36" s="12">
         <v>0</v>
       </c>
-      <c r="G32">
-        <f>C32*D32*1000000000</f>
+      <c r="G36">
+        <f>C36*D36*1000000000</f>
         <v>0</v>
       </c>
-      <c r="H32" t="str">
-        <f>IF(G32&gt;F32,"N", "Y")</f>
+      <c r="H36" t="str">
+        <f>IF(G36&gt;F36,"N", "Y")</f>
         <v>Y</v>
       </c>
-      <c r="I32">
+      <c r="I36" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B37" t="s">
         <v>16</v>
       </c>
-      <c r="C33">
+      <c r="C37">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D37">
         <v>0</v>
       </c>
-      <c r="E33">
-        <f>C33*D33</f>
+      <c r="E37">
+        <f>C37*D37</f>
         <v>0</v>
       </c>
-      <c r="F33" s="12">
+      <c r="F37" s="12">
         <v>0</v>
       </c>
-      <c r="G33">
-        <f>C33*D33*1000000000</f>
+      <c r="G37">
+        <f>C37*D37*1000000000</f>
         <v>0</v>
       </c>
-      <c r="H33" t="str">
-        <f>IF(G33&gt;F33,"N", "Y")</f>
+      <c r="H37" t="str">
+        <f>IF(G37&gt;F37,"N", "Y")</f>
         <v>Y</v>
       </c>
-      <c r="I33">
+      <c r="I37" s="11">
         <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>0</v>
-      </c>
-      <c r="E34">
-        <f>C34*D34</f>
-        <v>0</v>
-      </c>
-      <c r="F34" s="12">
-        <v>0</v>
-      </c>
-      <c r="G34">
-        <f>C34*D34*1000000000</f>
-        <v>0</v>
-      </c>
-      <c r="H34" t="str">
-        <f>IF(G34&gt;F34,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <f>C38*D38</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <f>C38*D38*1000000000</f>
+        <v>0</v>
+      </c>
+      <c r="H38" t="str">
+        <f>IF(G38&gt;F38,"N", "Y")</f>
+        <v>Y</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="11"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>0.85</v>
+      </c>
+      <c r="F40" s="11"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B42" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C42" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="F42" s="12"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B43" t="s">
         <v>16</v>
       </c>
-      <c r="C39">
+      <c r="F43" s="12"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="12"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B40" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>6</v>
-      </c>
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-      <c r="C41">
-        <v>0.8</v>
-      </c>
-      <c r="D41" s="7">
-        <f>D49</f>
+      <c r="D45" s="7">
+        <f>D53</f>
         <v>2.9133633909999999</v>
       </c>
-      <c r="E41">
+      <c r="E45">
         <f>E21/($E$21+$E$22)</f>
         <v>0.81417044373974945</v>
       </c>
-      <c r="F41">
-        <f>E41*$B$36*1000000000</f>
+      <c r="F45" s="12">
+        <f>E45*$B$40*1000000000</f>
         <v>692044877.17878699</v>
       </c>
-      <c r="G41" s="7">
-        <f>C41*D41*1000000000</f>
+      <c r="G45" s="7">
+        <f>C45*D45*1000000000</f>
         <v>2330690712.8000002</v>
       </c>
-      <c r="H41" t="str">
-        <f>IF(G41&gt;F41,"N", "Y")</f>
+      <c r="H45" t="str">
+        <f>IF(G45&gt;F45,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I41">
-        <f>F41</f>
+      <c r="I45" s="11">
+        <f>F45</f>
         <v>692044877.17878699</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B46" t="s">
         <v>12</v>
       </c>
-      <c r="C42">
+      <c r="C46">
         <v>0.8</v>
       </c>
-      <c r="D42" s="7">
-        <f>D50</f>
+      <c r="D46" s="7">
+        <f>D54</f>
         <v>0.66495784800000002</v>
       </c>
-      <c r="E42">
+      <c r="E46">
         <f>E22/($E$21+$E$22)</f>
         <v>0.18582955626025058</v>
       </c>
-      <c r="F42">
-        <f>E42*$B$36*1000000000</f>
+      <c r="F46" s="12">
+        <f>E46*$B$40*1000000000</f>
         <v>157955122.82121298</v>
       </c>
-      <c r="G42" s="7">
-        <f>C42*D42*1000000000</f>
+      <c r="G46" s="7">
+        <f>C46*D46*1000000000</f>
         <v>531966278.39999998</v>
       </c>
-      <c r="H42" t="str">
-        <f>IF(G42&gt;F42,"N", "Y")</f>
+      <c r="H46" t="str">
+        <f>IF(G46&gt;F46,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I42">
-        <f>F42</f>
+      <c r="I46" s="11">
+        <f>F46</f>
         <v>157955122.82121298</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="11"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B48">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+      <c r="F48" s="11"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="F49" s="11"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>13</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B50" t="s">
         <v>14</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C50" t="s">
         <v>15</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D50" t="s">
         <v>33</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E50" t="s">
         <v>26</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F50" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G50" t="s">
         <v>34</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B51" t="s">
         <v>12</v>
       </c>
-      <c r="C47">
+      <c r="C51">
         <v>0.8</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D51" s="7">
         <f>SUM(F3:H3)</f>
         <v>1.2122617959999999</v>
       </c>
-      <c r="E47" s="8">
+      <c r="E51" s="8">
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="F47" s="12">
-        <f>E47*$B$8*1000000000+1150000000*0.85/2</f>
+      <c r="F51" s="12">
+        <f>E51*$B$48*1000000000+1150000000*0.85/2</f>
         <v>623508363.60022318</v>
       </c>
-      <c r="G47">
-        <f>C47*D47*1000000000</f>
+      <c r="G51">
+        <f>C51*D51*1000000000</f>
         <v>969809436.79999995</v>
       </c>
-      <c r="H47" t="str">
-        <f>IF(G47&gt;F47,"N", "Y")</f>
+      <c r="H51" t="str">
+        <f>IF(G51&gt;F51,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I47">
-        <f>F47</f>
+      <c r="I51" s="11">
+        <f>F51</f>
         <v>623508363.60022318</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B52" t="s">
         <v>12</v>
       </c>
-      <c r="C48">
+      <c r="C52">
         <v>0.8</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D52" s="7">
         <f>SUM(F4:H4)</f>
         <v>2.8558627890000006</v>
       </c>
-      <c r="E48" s="8">
+      <c r="E52" s="8">
         <f>K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="F48" s="12">
-        <f>E48*$B$8*1000000000+O4*1000000000/2</f>
+      <c r="F52" s="12">
+        <f>E52*$B$48*1000000000+O4*1000000000</f>
         <v>548885847.01730013</v>
       </c>
-      <c r="G48">
-        <f>C48*D48*1000000000</f>
+      <c r="G52">
+        <f>C52*D52*1000000000</f>
         <v>2284690231.2000003</v>
       </c>
-      <c r="H48" t="str">
-        <f>IF(G48&gt;F48,"N", "Y")</f>
+      <c r="H52" t="str">
+        <f>IF(G52&gt;F52,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I48">
-        <f t="shared" ref="I48:I50" si="8">F48</f>
+      <c r="I52" s="11">
+        <f t="shared" ref="I52:I54" si="10">F52</f>
         <v>548885847.01730013</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>6</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B53" t="s">
         <v>12</v>
       </c>
-      <c r="C49">
+      <c r="C53">
         <v>0.8</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D53" s="7">
         <f>SUM(F5:H5)</f>
         <v>2.9133633909999999</v>
       </c>
-      <c r="E49" s="8">
+      <c r="E53" s="8">
         <f>K5</f>
         <v>0.38100883182298734</v>
       </c>
-      <c r="F49" s="12">
-        <f>E49*$B$8*1000000000+O5*1000000000/2</f>
+      <c r="F53" s="12">
+        <f>E53*$B$48*1000000000+O5*1000000000</f>
         <v>559937241.62713218</v>
       </c>
-      <c r="G49">
-        <f>C49*D49*1000000000</f>
+      <c r="G53">
+        <f>C53*D53*1000000000</f>
         <v>2330690712.8000002</v>
       </c>
-      <c r="H49" t="str">
-        <f>IF(G49&gt;F49,"N", "Y")</f>
+      <c r="H53" t="str">
+        <f>IF(G53&gt;F53,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="8"/>
+      <c r="I53" s="11">
+        <f t="shared" si="10"/>
         <v>559937241.62713218</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>7</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B54" t="s">
         <v>12</v>
       </c>
-      <c r="C50">
+      <c r="C54">
         <v>0.8</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D54" s="7">
         <f>SUM(F6:H6)</f>
         <v>0.66495784800000002</v>
       </c>
-      <c r="E50" s="8">
+      <c r="E54" s="8">
         <f>K6</f>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="F50" s="12">
-        <f>E50*$B$8*1000000000</f>
+      <c r="F54" s="12">
+        <f>E54*$B$48*1000000000</f>
         <v>73918547.755344689</v>
       </c>
-      <c r="G50">
-        <f>C50*D50*1000000000</f>
+      <c r="G54">
+        <f>C54*D54*1000000000</f>
         <v>531966278.39999998</v>
       </c>
-      <c r="H50" t="str">
-        <f>IF(G50&gt;F50,"N", "Y")</f>
+      <c r="H54" t="str">
+        <f>IF(G54&gt;F54,"N", "Y")</f>
         <v>N</v>
       </c>
-      <c r="I50">
-        <f t="shared" si="8"/>
+      <c r="I54" s="11">
+        <f t="shared" si="10"/>
         <v>73918547.755344689</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54">
-        <v>0.8</v>
-      </c>
-      <c r="D54" t="s">
-        <v>33</v>
-      </c>
-      <c r="E54" t="s">
-        <v>26</v>
-      </c>
-      <c r="F54" t="s">
-        <v>38</v>
-      </c>
-      <c r="G54" t="s">
-        <v>34</v>
-      </c>
-      <c r="H54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="7">
-        <f>C19</f>
-        <v>0.8</v>
-      </c>
-      <c r="D55" s="7">
-        <f>D19</f>
-        <v>0.25821176254799999</v>
-      </c>
-      <c r="E55" s="8">
-        <f>D55/SUM($D$55:$D$58)</f>
-        <v>0.35627124688223982</v>
-      </c>
-      <c r="F55" s="13">
-        <f>E55*$B$16*1000000000</f>
-        <v>302830559.84990388</v>
-      </c>
-      <c r="G55" s="11">
-        <f>C55*D55*1000000000</f>
-        <v>206569410.03840002</v>
-      </c>
-      <c r="H55" t="str">
-        <f>IF(G55&gt;F55,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I55" s="17">
-        <f>G55</f>
-        <v>206569410.03840002</v>
-      </c>
-      <c r="K55" s="9">
-        <f>I55/G55*0.8</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="7">
-        <f t="shared" ref="C56:D62" si="9">C20</f>
-        <v>0.8</v>
-      </c>
-      <c r="D56" s="7">
-        <f t="shared" si="9"/>
-        <v>0.27987455332200001</v>
-      </c>
-      <c r="E56" s="8">
-        <f t="shared" ref="E56:E58" si="10">D56/SUM($D$55:$D$58)</f>
-        <v>0.38616078175022389</v>
-      </c>
-      <c r="F56" s="13">
-        <f>E56*$B$16*1000000000</f>
-        <v>328236664.48769027</v>
-      </c>
-      <c r="G56" s="11">
-        <f>C56*D56*1000000000</f>
-        <v>223899642.65760002</v>
-      </c>
-      <c r="H56" t="str">
-        <f>IF(G56&gt;F56,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I56" s="17">
-        <f t="shared" ref="I56:I58" si="11">G56</f>
-        <v>223899642.65760002</v>
-      </c>
-      <c r="K56" s="9">
-        <f t="shared" ref="K56:K62" si="12">I56/G56*0.8</f>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D57" s="7">
-        <f t="shared" si="9"/>
-        <v>0.16606171328700001</v>
-      </c>
-      <c r="E57" s="8">
-        <f t="shared" si="10"/>
-        <v>0.22912594325040658</v>
-      </c>
-      <c r="F57" s="13">
-        <f>E57*$B$16*1000000000</f>
-        <v>194757051.76284558</v>
-      </c>
-      <c r="G57" s="11">
-        <f>C57*D57*1000000000</f>
-        <v>132849370.6296</v>
-      </c>
-      <c r="H57" t="str">
-        <f>IF(G57&gt;F57,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I57" s="17">
-        <f t="shared" si="11"/>
-        <v>132849370.6296</v>
-      </c>
-      <c r="K57" s="9">
-        <f t="shared" si="12"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D58" s="7">
-        <f t="shared" si="9"/>
-        <v>2.0613693288000001E-2</v>
-      </c>
-      <c r="E58" s="8">
-        <f t="shared" si="10"/>
-        <v>2.8442028117129644E-2</v>
-      </c>
-      <c r="F58" s="13">
-        <f>E58*$B$16*1000000000</f>
-        <v>24175723.899560198</v>
-      </c>
-      <c r="G58" s="11">
-        <f>C58*D58*1000000000</f>
-        <v>16490954.630400002</v>
-      </c>
-      <c r="H58" t="str">
-        <f>IF(G58&gt;F58,"N", "Y")</f>
-        <v>Y</v>
-      </c>
-      <c r="I58" s="17">
-        <f t="shared" si="11"/>
-        <v>16490954.630400002</v>
-      </c>
-      <c r="K58" s="9">
-        <f t="shared" si="12"/>
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D59" s="7">
-        <f>D23</f>
-        <v>0.77948433482799995</v>
-      </c>
-      <c r="E59" s="8"/>
-      <c r="F59" s="13">
-        <f>F55-G55</f>
-        <v>96261149.811503857</v>
-      </c>
-      <c r="G59" s="11">
-        <f>C59*D59*1000000000</f>
-        <v>623587467.86240005</v>
-      </c>
-      <c r="H59" t="str">
-        <f>IF(G59&gt;F59,"N", "Y")</f>
-        <v>N</v>
-      </c>
-      <c r="I59" s="17">
-        <f>F59</f>
-        <v>96261149.811503857</v>
-      </c>
-      <c r="K59" s="9">
-        <f t="shared" si="12"/>
-        <v>0.12349337313205239</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D60" s="7">
-        <f t="shared" si="9"/>
-        <v>1.8962928918960003</v>
-      </c>
-      <c r="F60" s="13">
-        <f>F56-G56</f>
-        <v>104337021.83009025</v>
-      </c>
-      <c r="G60" s="11">
-        <f t="shared" ref="G60:G62" si="13">C60*D60*1000000000</f>
-        <v>1517034313.5168004</v>
-      </c>
-      <c r="H60" t="str">
-        <f t="shared" ref="H60:H62" si="14">IF(G60&gt;F60,"N", "Y")</f>
-        <v>N</v>
-      </c>
-      <c r="I60" s="17">
-        <f t="shared" ref="I60:I62" si="15">F60</f>
-        <v>104337021.83009025</v>
-      </c>
-      <c r="K60" s="9">
-        <f t="shared" si="12"/>
-        <v>5.5021575135352288E-2</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D61" s="7">
-        <f t="shared" si="9"/>
-        <v>1.8878594773679997</v>
-      </c>
-      <c r="F61" s="13">
-        <f>F57-G57</f>
-        <v>61907681.133245572</v>
-      </c>
-      <c r="G61" s="11">
-        <f t="shared" si="13"/>
-        <v>1510287581.8943999</v>
-      </c>
-      <c r="H61" t="str">
-        <f t="shared" si="14"/>
-        <v>N</v>
-      </c>
-      <c r="I61" s="17">
-        <f t="shared" si="15"/>
-        <v>61907681.133245572</v>
-      </c>
-      <c r="K61" s="9">
-        <f t="shared" si="12"/>
-        <v>3.2792526072732656E-2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="7">
-        <f t="shared" si="9"/>
-        <v>0.8</v>
-      </c>
-      <c r="D62" s="7">
-        <f t="shared" si="9"/>
-        <v>0.377696057664</v>
-      </c>
-      <c r="F62" s="13">
-        <f>F58-G58</f>
-        <v>7684769.2691601962</v>
-      </c>
-      <c r="G62" s="11">
-        <f t="shared" si="13"/>
-        <v>302156846.13120002</v>
-      </c>
-      <c r="H62" t="str">
-        <f t="shared" si="14"/>
-        <v>N</v>
-      </c>
-      <c r="I62" s="17">
-        <f t="shared" si="15"/>
-        <v>7684769.2691601962</v>
-      </c>
-      <c r="K62" s="9">
-        <f t="shared" si="12"/>
-        <v>2.0346437600353772E-2</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2693,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O62"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2715,17 +2473,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3019,11 +2777,11 @@
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <f>D11*$B$8*1000000000</f>
         <v>134758363.60022315</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="14">
         <f>E11/(C11*1000000000)</f>
         <v>0.11116275712463609</v>
       </c>
@@ -3047,11 +2805,11 @@
         <f t="shared" ref="D12:D14" si="2">K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <f>D12*$B$8*1000000000</f>
         <v>317465581.59489292</v>
       </c>
-      <c r="F12" s="15">
+      <c r="F12" s="14">
         <f>E12/(C12*1000000000)</f>
         <v>0.11116275712463609</v>
       </c>
@@ -3075,11 +2833,11 @@
         <f t="shared" si="2"/>
         <v>0.38100883182298734</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <f>D13*$B$8*1000000000</f>
         <v>323857507.04953927</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <f>E13/(C13*1000000000)</f>
         <v>0.11116275712463611</v>
       </c>
@@ -3103,11 +2861,11 @@
         <f t="shared" si="2"/>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <f>D14*$B$8*1000000000</f>
         <v>73918547.755344689</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="14">
         <f>E14/(C14*1000000000)</f>
         <v>0.11116275712463609</v>
       </c>
@@ -3125,12 +2883,12 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -3153,7 +2911,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -3168,11 +2926,11 @@
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <f>D19*$B$16*1000000000</f>
         <v>134758363.60022315</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="14">
         <f>E19/(C19*1000000000)</f>
         <v>0.5218908785194184</v>
       </c>
@@ -3181,7 +2939,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -3196,11 +2954,11 @@
         <f t="shared" ref="D20:D22" si="5">K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <f>C20*0.8*1000000000</f>
         <v>223899642.65760002</v>
       </c>
-      <c r="F20" s="15">
+      <c r="F20" s="14">
         <f>E20/(C20*1000000000)</f>
         <v>0.79999999999999993</v>
       </c>
@@ -3209,7 +2967,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -3224,11 +2982,11 @@
         <f t="shared" si="5"/>
         <v>0.38100883182298734</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="13">
         <f>C21*0.8*1000000000</f>
         <v>132849370.6296</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F21" s="14">
         <f>E21/(C21*1000000000)</f>
         <v>0.8</v>
       </c>
@@ -3237,7 +2995,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -3252,11 +3010,11 @@
         <f t="shared" si="5"/>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="13">
         <f>C22*0.8*1000000000</f>
         <v>16490954.630400002</v>
       </c>
-      <c r="F22" s="15">
+      <c r="F22" s="14">
         <f t="shared" ref="F22:F23" si="6">E22/(C22*1000000000)</f>
         <v>0.8</v>
       </c>
@@ -3265,7 +3023,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -3281,7 +3039,7 @@
         <f>E11-E19</f>
         <v>0</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F23" s="14">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -3290,7 +3048,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -3306,7 +3064,7 @@
         <f>E12-E20</f>
         <v>93565938.937292904</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="14">
         <f>E24/(C24*1000000000)</f>
         <v>4.9341501693729077E-2</v>
       </c>
@@ -3315,7 +3073,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -3331,7 +3089,7 @@
         <f>E13-E21</f>
         <v>191008136.41993928</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="14">
         <f>E25/(C25*1000000000)</f>
         <v>0.10117709432814216</v>
       </c>
@@ -3340,7 +3098,7 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -3356,7 +3114,7 @@
         <f>E14-E22</f>
         <v>57427593.124944687</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="14">
         <f>E26/(C26*1000000000)</f>
         <v>0.15204710761379595</v>
       </c>
@@ -3365,20 +3123,26 @@
         <v>NO</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28">
         <v>0.85</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -3401,670 +3165,670 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="7">
+        <f>C19</f>
+        <v>0.25821176254799999</v>
+      </c>
+      <c r="D31" s="8">
+        <f>C31/SUM($C$31:$C$34)</f>
+        <v>0.35627124688223982</v>
+      </c>
+      <c r="E31" s="13">
+        <f>C31*0.8*1000000000</f>
+        <v>206569410.03840002</v>
+      </c>
+      <c r="F31" s="14">
+        <f>E31/(C31*1000000000)</f>
+        <v>0.80000000000000016</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" ref="G31:G38" si="7">IF(F31&gt;1, "YES", "NO")</f>
+        <v>NO</v>
+      </c>
+      <c r="I31" s="13">
+        <f>D31*$B$28*1000000000</f>
+        <v>302830559.84990388</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="7">
+        <f>C20</f>
+        <v>0.27987455332200001</v>
+      </c>
+      <c r="D32" s="8">
+        <f>C32/SUM($C$31:$C$34)</f>
+        <v>0.38616078175022389</v>
+      </c>
+      <c r="E32" s="13">
+        <f>C32*0.8*1000000000</f>
+        <v>223899642.65760002</v>
+      </c>
+      <c r="F32" s="14">
+        <f t="shared" ref="F32:F34" si="8">E32/(C32*1000000000)</f>
+        <v>0.79999999999999993</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="I32" s="13">
+        <f>D32*$B$28*1000000000</f>
+        <v>328236664.48769027</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="7">
+        <f>C21</f>
+        <v>0.16606171328700001</v>
+      </c>
+      <c r="D33" s="8">
+        <f>C33/SUM($C$31:$C$34)</f>
+        <v>0.22912594325040658</v>
+      </c>
+      <c r="E33" s="13">
+        <f>C33*0.8*1000000000</f>
+        <v>132849370.6296</v>
+      </c>
+      <c r="F33" s="14">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="I33" s="13">
+        <f>D33*$B$28*1000000000</f>
+        <v>194757051.76284558</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" s="7">
+        <f>C22</f>
+        <v>2.0613693288000001E-2</v>
+      </c>
+      <c r="D34" s="8">
+        <f>C34/SUM($C$31:$C$34)</f>
+        <v>2.8442028117129644E-2</v>
+      </c>
+      <c r="E34" s="13">
+        <f>C34*0.8*1000000000</f>
+        <v>16490954.630400002</v>
+      </c>
+      <c r="F34" s="14">
+        <f t="shared" si="8"/>
+        <v>0.8</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+      <c r="I34" s="13">
+        <f>D34*$B$28*1000000000</f>
+        <v>24175723.899560198</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="7">
+        <f>C23</f>
+        <v>0.77948433482799995</v>
+      </c>
+      <c r="D35" s="8"/>
+      <c r="E35" s="10">
+        <f>I31-E31</f>
+        <v>96261149.811503857</v>
+      </c>
+      <c r="F35" s="14">
+        <f t="shared" ref="F35" si="9">E35/(C35*1000000000)</f>
+        <v>0.12349337313205239</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="7">
+        <f>C24</f>
+        <v>1.8962928918960003</v>
+      </c>
+      <c r="D36" s="8"/>
+      <c r="E36" s="10">
+        <f t="shared" ref="E36:E38" si="10">I32-E32</f>
+        <v>104337021.83009025</v>
+      </c>
+      <c r="F36" s="14">
+        <f>E36/(C36*1000000000)</f>
+        <v>5.5021575135352295E-2</v>
+      </c>
+      <c r="G36" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="7">
+        <f>C25</f>
+        <v>1.8878594773679997</v>
+      </c>
+      <c r="D37" s="8"/>
+      <c r="E37" s="10">
+        <f t="shared" si="10"/>
+        <v>61907681.133245572</v>
+      </c>
+      <c r="F37" s="14">
+        <f>E37/(C37*1000000000)</f>
+        <v>3.2792526072732656E-2</v>
+      </c>
+      <c r="G37" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="7">
+        <f>C26</f>
+        <v>0.377696057664</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="10">
+        <f t="shared" si="10"/>
+        <v>7684769.2691601962</v>
+      </c>
+      <c r="F38" s="14">
+        <f>E38/(C38*1000000000)</f>
+        <v>2.0346437600353772E-2</v>
+      </c>
+      <c r="G38" t="str">
+        <f t="shared" si="7"/>
+        <v>NO</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C42" t="s">
+        <v>33</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" t="s">
+        <v>15</v>
+      </c>
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C43" s="7">
         <f>C11</f>
         <v>1.2122617959999999</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D43" s="8">
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="E31" s="14">
-        <f>B28*1000000000</f>
+      <c r="E43" s="13">
+        <f>B40*1000000000</f>
         <v>850000000</v>
       </c>
-      <c r="F31" s="15">
-        <f t="shared" ref="F31:F34" si="7">E31/(C31*1000000000)</f>
+      <c r="F43" s="14">
+        <f t="shared" ref="F43:F46" si="11">E43/(C43*1000000000)</f>
         <v>0.70116867726482413</v>
       </c>
-      <c r="G31" t="str">
-        <f t="shared" ref="G31:G34" si="8">IF(F31&gt;1, "YES", "NO")</f>
+      <c r="G43" t="str">
+        <f t="shared" ref="G43:G46" si="12">IF(F43&gt;1, "YES", "NO")</f>
         <v>NO</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>5</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B44" t="s">
         <v>12</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C44" s="7">
         <f>C12</f>
         <v>2.8558627890000006</v>
       </c>
-      <c r="D32" s="8">
-        <f t="shared" ref="D32:D34" si="9">K4</f>
+      <c r="D44" s="8">
+        <f>K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E44" s="13">
         <v>0</v>
       </c>
-      <c r="F32" s="15">
-        <f t="shared" si="7"/>
+      <c r="F44" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G32" t="str">
-        <f t="shared" si="8"/>
+      <c r="G44" t="str">
+        <f t="shared" si="12"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>6</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B45" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C45" s="7">
         <f>C13</f>
         <v>2.9133633909999999</v>
       </c>
-      <c r="D33" s="8">
-        <f t="shared" si="9"/>
+      <c r="D45" s="8">
+        <f>K5</f>
         <v>0.38100883182298734</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E45" s="13">
         <v>0</v>
       </c>
-      <c r="F33" s="15">
-        <f t="shared" si="7"/>
+      <c r="F45" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G33" t="str">
-        <f t="shared" si="8"/>
+      <c r="G45" t="str">
+        <f t="shared" si="12"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>7</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B46" t="s">
         <v>12</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C46" s="7">
         <f>C14</f>
         <v>0.66495784800000002</v>
       </c>
-      <c r="D34" s="8">
-        <f t="shared" si="9"/>
+      <c r="D46" s="8">
+        <f>K6</f>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E46" s="13">
         <v>0</v>
       </c>
-      <c r="F34" s="15">
-        <f t="shared" si="7"/>
+      <c r="F46" s="14">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G34" t="str">
-        <f t="shared" si="8"/>
+      <c r="G46" t="str">
+        <f t="shared" si="12"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B36">
+      <c r="B48">
         <v>0.85</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>13</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B50" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C50" t="s">
         <v>33</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D50" t="s">
         <v>26</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E50" t="s">
         <v>27</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F50" t="s">
         <v>15</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G50" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>4</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B51" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="7">
-        <f>C31</f>
+      <c r="C51" s="7">
+        <f>C43</f>
         <v>1.2122617959999999</v>
       </c>
-      <c r="D39" s="8">
+      <c r="D51" s="8">
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E51" s="13">
         <v>0</v>
       </c>
-      <c r="F39" s="15">
-        <f t="shared" ref="F39:F42" si="10">E39/(C39*1000000000)</f>
+      <c r="F51" s="14">
+        <f t="shared" ref="F51:F54" si="13">E51/(C51*1000000000)</f>
         <v>0</v>
       </c>
-      <c r="G39" t="str">
-        <f t="shared" ref="G39:G42" si="11">IF(F39&gt;1, "YES", "NO")</f>
+      <c r="G51" t="str">
+        <f t="shared" ref="G51:G54" si="14">IF(F51&gt;1, "YES", "NO")</f>
         <v>NO</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>5</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B52" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="7">
-        <f t="shared" ref="C40:C42" si="12">C32</f>
+      <c r="C52" s="7">
+        <f t="shared" ref="C52:C54" si="15">C44</f>
         <v>2.8558627890000006</v>
       </c>
-      <c r="D40" s="8">
-        <f t="shared" ref="D40:D41" si="13">K4</f>
+      <c r="D52" s="8">
+        <f>K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E52" s="13">
         <v>0</v>
       </c>
-      <c r="F40" s="15">
-        <f t="shared" si="10"/>
+      <c r="F52" s="14">
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G40" t="str">
-        <f t="shared" si="11"/>
+      <c r="G52" t="str">
+        <f t="shared" si="14"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>6</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B53" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="7">
-        <f t="shared" si="12"/>
+      <c r="C53" s="7">
+        <f t="shared" si="15"/>
         <v>2.9133633909999999</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D53" s="8">
+        <f>K5</f>
+        <v>0.38100883182298734</v>
+      </c>
+      <c r="E53" s="13">
+        <f>$B$48*(K5/($K$6+$K$5))*1000000000</f>
+        <v>692044877.17878699</v>
+      </c>
+      <c r="F53" s="14">
         <f t="shared" si="13"/>
-        <v>0.38100883182298734</v>
-      </c>
-      <c r="E41" s="14">
-        <f>$B$36*(K5/($K$6+$K$5))*1000000000</f>
-        <v>692044877.17878699</v>
-      </c>
-      <c r="F41" s="15">
-        <f t="shared" si="10"/>
         <v>0.23754155740291821</v>
       </c>
-      <c r="G41" t="str">
-        <f t="shared" si="11"/>
+      <c r="G53" t="str">
+        <f t="shared" si="14"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>7</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B54" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="7">
-        <f t="shared" si="12"/>
+      <c r="C54" s="7">
+        <f t="shared" si="15"/>
         <v>0.66495784800000002</v>
       </c>
-      <c r="D42" s="8">
+      <c r="D54" s="8">
         <f>K6</f>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="E42" s="14">
-        <f>$B$36*(K6/($K$6+$K$5))*1000000000</f>
+      <c r="E54" s="13">
+        <f>$B$48*(K6/($K$6+$K$5))*1000000000</f>
         <v>157955122.82121298</v>
       </c>
-      <c r="F42" s="15">
-        <f t="shared" si="10"/>
+      <c r="F54" s="14">
+        <f t="shared" si="13"/>
         <v>0.23754155740291824</v>
       </c>
-      <c r="G42" t="str">
-        <f t="shared" si="11"/>
+      <c r="G54" t="str">
+        <f t="shared" si="14"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B56">
         <v>0.85</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>13</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B58" t="s">
         <v>14</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C58" t="s">
         <v>33</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D58" t="s">
         <v>26</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F58" t="s">
         <v>15</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G58" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>4</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B59" t="s">
         <v>12</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C59" s="7">
         <f>SUM(F3:H3)</f>
         <v>1.2122617959999999</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D59" s="8">
         <f>K3</f>
         <v>0.15853925129438018</v>
       </c>
-      <c r="E47" s="16">
-        <f>D47*$B$8*1000000000+1150000000*0.85/2</f>
+      <c r="E59" s="15">
+        <f>D59*$B$8*1000000000+1150000000*0.85/2</f>
         <v>623508363.60022318</v>
       </c>
-      <c r="F47" s="15">
-        <f t="shared" ref="F47:F50" si="14">E47/(C47*1000000000)</f>
+      <c r="F59" s="14">
+        <f t="shared" ref="F59:F62" si="16">E59/(C59*1000000000)</f>
         <v>0.51433474655190992</v>
       </c>
-      <c r="G47" t="str">
-        <f t="shared" ref="G47:G50" si="15">IF(F47&gt;1, "YES", "NO")</f>
+      <c r="G59" t="str">
+        <f t="shared" ref="G59:G62" si="17">IF(F59&gt;1, "YES", "NO")</f>
         <v>NO</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>5</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B60" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="7">
+      <c r="C60" s="7">
         <f>SUM(F4:H4)</f>
         <v>2.8558627890000006</v>
       </c>
-      <c r="D48" s="8">
+      <c r="D60" s="8">
         <f>K4</f>
         <v>0.37348891952340341</v>
       </c>
-      <c r="E48" s="16">
-        <f>D48*$B$8*1000000000+O4*1000000000/2</f>
+      <c r="E60" s="15">
+        <f>D60*$B$8*1000000000+O4*1000000000/2</f>
         <v>548885847.01730013</v>
       </c>
-      <c r="F48" s="15">
-        <f t="shared" si="14"/>
+      <c r="F60" s="14">
+        <f t="shared" si="16"/>
         <v>0.19219615491733627</v>
       </c>
-      <c r="G48" t="str">
-        <f t="shared" si="15"/>
+      <c r="G60" t="str">
+        <f t="shared" si="17"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>6</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B61" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="7">
+      <c r="C61" s="7">
         <f>SUM(F5:H5)</f>
         <v>2.9133633909999999</v>
       </c>
-      <c r="D49" s="8">
+      <c r="D61" s="8">
         <f>K5</f>
         <v>0.38100883182298734</v>
       </c>
-      <c r="E49" s="16">
-        <f>D49*$B$8*1000000000+O5*1000000000/2</f>
+      <c r="E61" s="15">
+        <f>D61*$B$8*1000000000+O5*1000000000/2</f>
         <v>559937241.62713218</v>
       </c>
-      <c r="F49" s="15">
-        <f t="shared" si="14"/>
+      <c r="F61" s="14">
+        <f t="shared" si="16"/>
         <v>0.1921961549173363</v>
       </c>
-      <c r="G49" t="str">
-        <f t="shared" si="15"/>
+      <c r="G61" t="str">
+        <f t="shared" si="17"/>
         <v>NO</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>7</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B62" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C62" s="7">
         <f>SUM(F6:H6)</f>
         <v>0.66495784800000002</v>
       </c>
-      <c r="D50" s="8">
+      <c r="D62" s="8">
         <f>K6</f>
         <v>8.6962997359229049E-2</v>
       </c>
-      <c r="E50" s="16">
-        <f>D50*$B$8*1000000000</f>
+      <c r="E62" s="15">
+        <f>D62*$B$8*1000000000</f>
         <v>73918547.755344689</v>
       </c>
-      <c r="F50" s="15">
-        <f t="shared" si="14"/>
+      <c r="F62" s="14">
+        <f t="shared" si="16"/>
         <v>0.11116275712463609</v>
       </c>
-      <c r="G50" t="str">
-        <f t="shared" si="15"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" t="s">
-        <v>14</v>
-      </c>
-      <c r="C54" t="s">
-        <v>33</v>
-      </c>
-      <c r="D54" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54" t="s">
-        <v>27</v>
-      </c>
-      <c r="F54" t="s">
-        <v>15</v>
-      </c>
-      <c r="G54" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" t="s">
-        <v>32</v>
-      </c>
-      <c r="C55" s="7">
-        <f>C19</f>
-        <v>0.25821176254799999</v>
-      </c>
-      <c r="D55" s="8">
-        <f>C55/SUM($C$55:$C$58)</f>
-        <v>0.35627124688223982</v>
-      </c>
-      <c r="E55" s="14">
-        <f>C55*0.8*1000000000</f>
-        <v>206569410.03840002</v>
-      </c>
-      <c r="F55" s="15">
-        <f>E55/(C55*1000000000)</f>
-        <v>0.80000000000000016</v>
-      </c>
-      <c r="G55" t="str">
-        <f t="shared" ref="G55:G62" si="16">IF(F55&gt;1, "YES", "NO")</f>
-        <v>NO</v>
-      </c>
-      <c r="I55" s="14">
-        <f>D55*$B$52*1000000000</f>
-        <v>302830559.84990388</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" t="s">
-        <v>32</v>
-      </c>
-      <c r="C56" s="7">
-        <f t="shared" ref="C56:C62" si="17">C20</f>
-        <v>0.27987455332200001</v>
-      </c>
-      <c r="D56" s="8">
-        <f t="shared" ref="D56:D58" si="18">C56/SUM($C$55:$C$58)</f>
-        <v>0.38616078175022389</v>
-      </c>
-      <c r="E56" s="14">
-        <f>C56*0.8*1000000000</f>
-        <v>223899642.65760002</v>
-      </c>
-      <c r="F56" s="15">
-        <f t="shared" ref="F56:F58" si="19">E56/(C56*1000000000)</f>
-        <v>0.79999999999999993</v>
-      </c>
-      <c r="G56" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-      <c r="I56" s="14">
-        <f>D56*$B$52*1000000000</f>
-        <v>328236664.48769027</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>6</v>
-      </c>
-      <c r="B57" t="s">
-        <v>32</v>
-      </c>
-      <c r="C57" s="7">
+      <c r="G62" t="str">
         <f t="shared" si="17"/>
-        <v>0.16606171328700001</v>
-      </c>
-      <c r="D57" s="8">
-        <f t="shared" si="18"/>
-        <v>0.22912594325040658</v>
-      </c>
-      <c r="E57" s="14">
-        <f>C57*0.8*1000000000</f>
-        <v>132849370.6296</v>
-      </c>
-      <c r="F57" s="15">
-        <f t="shared" si="19"/>
-        <v>0.8</v>
-      </c>
-      <c r="G57" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-      <c r="I57" s="14">
-        <f>D57*$B$52*1000000000</f>
-        <v>194757051.76284558</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>7</v>
-      </c>
-      <c r="B58" t="s">
-        <v>32</v>
-      </c>
-      <c r="C58" s="7">
-        <f t="shared" si="17"/>
-        <v>2.0613693288000001E-2</v>
-      </c>
-      <c r="D58" s="8">
-        <f t="shared" si="18"/>
-        <v>2.8442028117129644E-2</v>
-      </c>
-      <c r="E58" s="14">
-        <f>C58*0.8*1000000000</f>
-        <v>16490954.630400002</v>
-      </c>
-      <c r="F58" s="15">
-        <f t="shared" si="19"/>
-        <v>0.8</v>
-      </c>
-      <c r="G58" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-      <c r="I58" s="14">
-        <f>D58*$B$52*1000000000</f>
-        <v>24175723.899560198</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>4</v>
-      </c>
-      <c r="B59" t="s">
-        <v>36</v>
-      </c>
-      <c r="C59" s="7">
-        <f t="shared" si="17"/>
-        <v>0.77948433482799995</v>
-      </c>
-      <c r="D59" s="8"/>
-      <c r="E59" s="10">
-        <f>I55-E55</f>
-        <v>96261149.811503857</v>
-      </c>
-      <c r="F59" s="15">
-        <f t="shared" ref="F59" si="20">E59/(C59*1000000000)</f>
-        <v>0.12349337313205239</v>
-      </c>
-      <c r="G59" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" t="s">
-        <v>36</v>
-      </c>
-      <c r="C60" s="7">
-        <f t="shared" si="17"/>
-        <v>1.8962928918960003</v>
-      </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="10">
-        <f t="shared" ref="E60:E62" si="21">I56-E56</f>
-        <v>104337021.83009025</v>
-      </c>
-      <c r="F60" s="15">
-        <f>E60/(C60*1000000000)</f>
-        <v>5.5021575135352295E-2</v>
-      </c>
-      <c r="G60" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>6</v>
-      </c>
-      <c r="B61" t="s">
-        <v>36</v>
-      </c>
-      <c r="C61" s="7">
-        <f t="shared" si="17"/>
-        <v>1.8878594773679997</v>
-      </c>
-      <c r="D61" s="8"/>
-      <c r="E61" s="10">
-        <f t="shared" si="21"/>
-        <v>61907681.133245572</v>
-      </c>
-      <c r="F61" s="15">
-        <f>E61/(C61*1000000000)</f>
-        <v>3.2792526072732656E-2</v>
-      </c>
-      <c r="G61" t="str">
-        <f t="shared" si="16"/>
-        <v>NO</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>7</v>
-      </c>
-      <c r="B62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" s="7">
-        <f t="shared" si="17"/>
-        <v>0.377696057664</v>
-      </c>
-      <c r="D62" s="8"/>
-      <c r="E62" s="10">
-        <f t="shared" si="21"/>
-        <v>7684769.2691601962</v>
-      </c>
-      <c r="F62" s="15">
-        <f>E62/(C62*1000000000)</f>
-        <v>2.0346437600353772E-2</v>
-      </c>
-      <c r="G62" t="str">
-        <f t="shared" si="16"/>
         <v>NO</v>
       </c>
     </row>

</xml_diff>